<commit_message>
returning errors by logs, it still needs revsion. Load/upload data
</commit_message>
<xml_diff>
--- a/storage/app/public/users/jose.jdgo97/LIQUIDACION.xlsx
+++ b/storage/app/public/users/jose.jdgo97/LIQUIDACION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\www\LARAVEL\REPOSITORIOS - DOWNLOADS\multimedia_cam\public\storage\users\jose.jdgo97\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEF1544-1AF5-44E9-A1D6-F414324A2247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29F8183-EFF3-4748-89CC-B1518C3F474B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1089,7 +1089,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:I9"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1275,7 +1275,7 @@
         <v>45736</v>
       </c>
       <c r="I7" s="4">
-        <v>45741</v>
+        <v>45742</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>32</v>

</xml_diff>